<commit_message>
Forwarding to the right area while getting row ticket
</commit_message>
<xml_diff>
--- a/Labels.xlsx
+++ b/Labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adval\OneDrive\Desktop\TRIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFC9C77-BCB2-451A-A06D-8B31A67342FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962EAC1D-5E38-4EE6-AC88-4F3F7E37AD59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{45465FF2-9264-4E7D-A38B-83046E50FA28}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
   <si>
     <t>Importance</t>
   </si>
@@ -526,6 +526,15 @@
   </si>
   <si>
     <t>Successful</t>
+  </si>
+  <si>
+    <t>a1.9</t>
+  </si>
+  <si>
+    <t>b1.9</t>
+  </si>
+  <si>
+    <t>Forwarding to the right area while getting row ticket</t>
   </si>
 </sst>
 </file>
@@ -877,9 +886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3423CBA-03A9-4BEF-8CE5-82753D13536A}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1030,617 +1041,631 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
         <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
         <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
         <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
         <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
         <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
         <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
         <v>80</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
         <v>80</v>
       </c>
       <c r="D34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
         <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
         <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
         <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
         <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
         <v>80</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s">
         <v>80</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
         <v>80</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
         <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
         <v>132</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
         <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
         <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C47" t="s">
         <v>132</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C48" t="s">
         <v>132</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C49" t="s">
         <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C50" t="s">
         <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B51" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C51" t="s">
         <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C52" t="s">
         <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C53" t="s">
         <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B54" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
         <v>132</v>
       </c>
       <c r="D54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+      <c r="D55" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>